<commit_message>
add save in xlsx all & one
</commit_message>
<xml_diff>
--- a/public/Excel/путевой_лист.xlsx
+++ b/public/Excel/путевой_лист.xlsx
@@ -46,7 +46,7 @@
     <t>N</t>
   </si>
   <si>
-    <t>05</t>
+    <t>01</t>
   </si>
   <si>
     <t>России от 28.11.97 N 78</t>
@@ -159,7 +159,7 @@
     <t>192289, Р.Ф., г. Санкт-Петербург, Грузовой проезд, дом 16, +7 (812) 333-28-25</t>
   </si>
   <si>
-    <t>ВКЖ</t>
+    <t>Пропек ветеранов 169к1</t>
   </si>
   <si>
     <t>Бригада</t>
@@ -171,19 +171,19 @@
     <t xml:space="preserve">Марка автобуса </t>
   </si>
   <si>
-    <t>Волга</t>
+    <t>ВАЗ</t>
   </si>
   <si>
     <t>Автобус</t>
   </si>
   <si>
-    <t>Рихарда Зорге</t>
+    <t>Говорова 37</t>
   </si>
   <si>
     <t xml:space="preserve">Государственный номерной знак </t>
   </si>
   <si>
-    <t>rwrwr</t>
+    <t>п555ее</t>
   </si>
   <si>
     <t>Гаражный номер</t>
@@ -198,7 +198,7 @@
     <t xml:space="preserve">Водитель </t>
   </si>
   <si>
-    <t>олег Петров</t>
+    <t>IGOR PETROV</t>
   </si>
   <si>
     <t>Табельный номер</t>
@@ -625,7 +625,7 @@
     <t>Выезд разрешен. Механик</t>
   </si>
   <si>
-    <t>Саныч</t>
+    <t>Михалыч</t>
   </si>
   <si>
     <t>21</t>
@@ -671,7 +671,7 @@
     <t>Диспетчер</t>
   </si>
   <si>
-    <t>Петрович</t>
+    <t>Иванов Иван</t>
   </si>
   <si>
     <t>К оплате,
@@ -2512,7 +2512,7 @@
       <c r="R3" s="167"/>
       <c r="S3" s="167"/>
       <c r="T3" s="170">
-        <v>16032113</v>
+        <v>16032112</v>
       </c>
       <c r="U3" s="170"/>
       <c r="V3" s="170"/>
@@ -2553,7 +2553,7 @@
       <c r="AY3" s="172"/>
       <c r="AZ3" s="172"/>
       <c r="BA3" s="173">
-        <v>16032113</v>
+        <v>16032112</v>
       </c>
       <c r="BB3" s="173"/>
       <c r="BC3" s="173"/>
@@ -2575,7 +2575,7 @@
       <c r="BQ3" s="172"/>
       <c r="BR3" s="172"/>
       <c r="BS3" s="173">
-        <v>16032113</v>
+        <v>16032112</v>
       </c>
       <c r="BT3" s="173"/>
       <c r="BU3" s="173"/>
@@ -4104,7 +4104,7 @@
       <c r="F15" s="66"/>
       <c r="G15" s="66"/>
       <c r="H15" s="67">
-        <v>13131313</v>
+        <v>24243452</v>
       </c>
       <c r="I15" s="67"/>
       <c r="J15" s="67"/>

</xml_diff>